<commit_message>
Updated the verify, verifyWithScreen methods in UtilityMethods. Updated variables report, test, driver in setting to static.
</commit_message>
<xml_diff>
--- a/OrionProjectsWorkingCopy/DataFiles/Dev/Platform.xlsx
+++ b/OrionProjectsWorkingCopy/DataFiles/Dev/Platform.xlsx
@@ -1,26 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rv042687/git/SeleniumV21Dec2016/OrionProjectsWorkingCopy/DataFiles/Dev/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18345" windowHeight="3270" tabRatio="500"/>
+    <workbookView xWindow="4420" yWindow="4180" windowWidth="23980" windowHeight="7860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="PatientSearch" sheetId="2" r:id="rId1"/>
+    <sheet name="Chart" sheetId="4" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>ORN_VR_PatientSearch</t>
   </si>
@@ -31,74 +39,95 @@
     <t>URL</t>
   </si>
   <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>jw027642</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>PatientSearchString1</t>
+  </si>
+  <si>
+    <t>PatientSearchString3</t>
+  </si>
+  <si>
+    <t>PatientSearchString2</t>
+  </si>
+  <si>
+    <t>Vader, Darth</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>SearchStringType1</t>
+  </si>
+  <si>
+    <t>FIN</t>
+  </si>
+  <si>
+    <t>ExpectedFullName2</t>
+  </si>
+  <si>
+    <t>SearchStringType2</t>
+  </si>
+  <si>
+    <t>SearchStringType3</t>
+  </si>
+  <si>
+    <t>ExpectedFullName3</t>
+  </si>
+  <si>
+    <t>ExpectedEncounterFIN3</t>
+  </si>
+  <si>
+    <t>MRN</t>
+  </si>
+  <si>
+    <t>ExpectedFullName1</t>
+  </si>
+  <si>
+    <t>Hanks, Lorrie</t>
+  </si>
+  <si>
+    <t>THOMAS, FRANK</t>
+  </si>
+  <si>
+    <t>https://ion-visit-list.test.devcernerpowerchart.com/search/patients</t>
+  </si>
+  <si>
+    <t>TestCase</t>
+  </si>
+  <si>
+    <t>ORN_VR_VisitList</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>PatientA</t>
+  </si>
+  <si>
+    <t>PatientB</t>
+  </si>
+  <si>
+    <t>DODDS, BRIAN</t>
+  </si>
+  <si>
     <t>https://deveng.test.devcernerpowerchart.com/search/patients</t>
-  </si>
-  <si>
-    <t>Username</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>jw027642</t>
-  </si>
-  <si>
-    <t>asdf</t>
-  </si>
-  <si>
-    <t>PatientSearchString1</t>
-  </si>
-  <si>
-    <t>PatientSearchString3</t>
-  </si>
-  <si>
-    <t>PatientSearchString2</t>
-  </si>
-  <si>
-    <t>Vader, Darth</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>SearchStringType1</t>
-  </si>
-  <si>
-    <t>FIN</t>
-  </si>
-  <si>
-    <t>ExpectedFullName2</t>
-  </si>
-  <si>
-    <t>SearchStringType2</t>
-  </si>
-  <si>
-    <t>SearchStringType3</t>
-  </si>
-  <si>
-    <t>ExpectedFullName3</t>
-  </si>
-  <si>
-    <t>ExpectedEncounterFIN3</t>
-  </si>
-  <si>
-    <t>MRN</t>
-  </si>
-  <si>
-    <t>ExpectedFullName1</t>
-  </si>
-  <si>
-    <t>Hanks, Lorrie</t>
-  </si>
-  <si>
-    <t>THOMAS, FRANK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,8 +135,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -117,6 +154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -133,7 +176,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -144,6 +187,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,23 +471,23 @@
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="66.75" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.75" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.25" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.875" style="2" customWidth="1"/>
-    <col min="7" max="8" width="19.75" style="2" customWidth="1"/>
-    <col min="9" max="9" width="21.375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="19.83203125" style="2" customWidth="1"/>
+    <col min="7" max="8" width="19.6640625" style="2" customWidth="1"/>
+    <col min="9" max="9" width="21.33203125" style="2" customWidth="1"/>
     <col min="10" max="10" width="21.5" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.25" style="2" customWidth="1"/>
-    <col min="12" max="13" width="16.875" style="2" customWidth="1"/>
-    <col min="14" max="14" width="22.625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.1640625" style="2" customWidth="1"/>
+    <col min="12" max="13" width="16.83203125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="22.6640625" style="2" customWidth="1"/>
     <col min="15" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
@@ -455,84 +499,150 @@
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="2" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="G2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="2">
         <v>20000019</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" s="2">
         <v>10001080</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N2" s="2">
         <v>20001330</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
+    <col min="2" max="2" width="57" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="17" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>1234567</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Worked on Visit List Test Plan
</commit_message>
<xml_diff>
--- a/OrionProjectsWorkingCopy/DataFiles/Dev/Platform.xlsx
+++ b/OrionProjectsWorkingCopy/DataFiles/Dev/Platform.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4420" yWindow="4180" windowWidth="23980" windowHeight="7860" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PatientSearch" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
   <si>
     <t>ORN_VR_PatientSearch</t>
   </si>
@@ -121,6 +121,45 @@
   </si>
   <si>
     <t>https://deveng.test.devcernerpowerchart.com/search/patients</t>
+  </si>
+  <si>
+    <t>Enc1_Time</t>
+  </si>
+  <si>
+    <t>Enc1_AttPhy</t>
+  </si>
+  <si>
+    <t>Enc1_Type</t>
+  </si>
+  <si>
+    <t>Enc1_Reason</t>
+  </si>
+  <si>
+    <t>Enc2_Time</t>
+  </si>
+  <si>
+    <t>Enc2_AttPhy</t>
+  </si>
+  <si>
+    <t>Enc2_Type</t>
+  </si>
+  <si>
+    <t>Enc2_Reason</t>
+  </si>
+  <si>
+    <t>Enc3_Time</t>
+  </si>
+  <si>
+    <t>Enc3_AttPhy</t>
+  </si>
+  <si>
+    <t>Enc3_Type</t>
+  </si>
+  <si>
+    <t>Enc3_Reason</t>
+  </si>
+  <si>
+    <t>Chest pain</t>
   </si>
 </sst>
 </file>
@@ -144,7 +183,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +202,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -176,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -188,6 +233,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -470,7 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -586,10 +633,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -600,9 +647,17 @@
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="15.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.5" customWidth="1"/>
+    <col min="13" max="13" width="13.5" customWidth="1"/>
+    <col min="14" max="15" width="12.83203125" customWidth="1"/>
+    <col min="16" max="16" width="17.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+    <col min="19" max="19" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -624,8 +679,44 @@
       <c r="G1" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="H1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -643,6 +734,9 @@
       </c>
       <c r="G2">
         <v>1234567</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated VisitList Test Plan
</commit_message>
<xml_diff>
--- a/OrionProjectsWorkingCopy/DataFiles/Dev/Platform.xlsx
+++ b/OrionProjectsWorkingCopy/DataFiles/Dev/Platform.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="37760" yWindow="5000" windowWidth="28800" windowHeight="16300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="PatientSearch" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="49">
   <si>
     <t>ORN_VR_PatientSearch</t>
   </si>
@@ -160,6 +160,21 @@
   </si>
   <si>
     <t>Chest pain</t>
+  </si>
+  <si>
+    <t>FINA</t>
+  </si>
+  <si>
+    <t>Kheang, NoEncntr2</t>
+  </si>
+  <si>
+    <t>FINB</t>
+  </si>
+  <si>
+    <t>RelationType</t>
+  </si>
+  <si>
+    <t>Admitting Physician</t>
   </si>
 </sst>
 </file>
@@ -633,10 +648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -647,17 +662,19 @@
     <col min="4" max="4" width="11.83203125" customWidth="1"/>
     <col min="5" max="5" width="17" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
-    <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
-    <col min="11" max="11" width="12.5" customWidth="1"/>
-    <col min="13" max="13" width="13.5" customWidth="1"/>
-    <col min="14" max="15" width="12.83203125" customWidth="1"/>
-    <col min="16" max="16" width="17.6640625" customWidth="1"/>
-    <col min="17" max="17" width="15.33203125" customWidth="1"/>
-    <col min="19" max="19" width="13" customWidth="1"/>
+    <col min="7" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="24.5" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.5" customWidth="1"/>
+    <col min="14" max="14" width="13.5" customWidth="1"/>
+    <col min="15" max="16" width="12.83203125" customWidth="1"/>
+    <col min="17" max="17" width="17.6640625" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" customWidth="1"/>
+    <col min="20" max="20" width="13" customWidth="1"/>
+    <col min="21" max="21" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -674,49 +691,55 @@
         <v>27</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="G1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="R1" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="S1" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="T1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="U1" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -732,10 +755,19 @@
       <c r="E2" t="s">
         <v>29</v>
       </c>
-      <c r="G2">
+      <c r="F2">
         <v>1234567</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2">
+        <v>20001379</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" t="s">
         <v>43</v>
       </c>
     </row>

</xml_diff>